<commit_message>
Hallituspalautteen viestejä muotoiltu uudestaan.
</commit_message>
<xml_diff>
--- a/hallituspalaute.xlsx
+++ b/hallituspalaute.xlsx
@@ -1,41 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samu\Documents\koodi\TGbot\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10176" windowHeight="5748"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Taul1" sheetId="1" r:id="rId1"/>
+    <sheet name="Taul1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2">
+  <si>
+    <t>Töttöröö 31.3.2017 @ 14:50</t>
+  </si>
+  <si>
+    <t>En ole tyytyväinen. 31.3.2017 @ 14:53</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -51,24 +54,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normaali" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normaali" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -368,15 +362,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A2:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Lisätty odotettavien_listaan lisäyksen aikaleima
</commit_message>
<xml_diff>
--- a/hallituspalaute.xlsx
+++ b/hallituspalaute.xlsx
@@ -1,44 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samu\Documents\koodi\TGbot\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10176" windowHeight="5748"/>
   </bookViews>
   <sheets>
-    <sheet name="Taul1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Taul1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2">
-  <si>
-    <t>Töttöröö 31.3.2017 @ 14:50</t>
-  </si>
-  <si>
-    <t>En ole tyytyväinen. 31.3.2017 @ 14:53</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -54,15 +51,24 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normaali" xfId="0"/>
+    <cellStyle name="Normaali" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -362,30 +368,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A2:A3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
-  <sheetData>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Hätäinen push, toivottavasti kääntyy
</commit_message>
<xml_diff>
--- a/hallituspalaute.xlsx
+++ b/hallituspalaute.xlsx
@@ -1,41 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samu\Documents\koodi\TGbot\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10176" windowHeight="5748"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Taul1" sheetId="1" r:id="rId1"/>
+    <sheet name="Taul1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1">
+  <si>
+    <t>moi 1.4.2017 @ 20:0</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -51,24 +51,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normaali" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normaali" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -368,15 +359,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A2:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
RPi GPIO import ovianturiin
</commit_message>
<xml_diff>
--- a/hallituspalaute.xlsx
+++ b/hallituspalaute.xlsx
@@ -14,9 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2">
   <si>
     <t>moi 1.4.2017 @ 20:0</t>
+  </si>
+  <si>
+    <t>Testi 7.4.2017 @ 21:47</t>
   </si>
 </sst>
 </file>
@@ -364,7 +367,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:A2"/>
+  <dimension ref="A2:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
@@ -377,6 +380,11 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Lisätty hallituspalautteen aikakatkaisu, jotta chat_id:t eivät roiku odotettavien_listalla turhaan.
</commit_message>
<xml_diff>
--- a/hallituspalaute.xlsx
+++ b/hallituspalaute.xlsx
@@ -14,12 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3">
   <si>
     <t>moi 1.4.2017 @ 20:0</t>
   </si>
   <si>
     <t>Testi 7.4.2017 @ 21:47</t>
+  </si>
+  <si>
+    <t>En tykkää :( 10.4.2017 @ 14:4</t>
   </si>
 </sst>
 </file>
@@ -367,7 +370,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:A3"/>
+  <dimension ref="A2:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
@@ -385,6 +388,11 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Śiirretty nakkikone omaksi moduulikseen.
</commit_message>
<xml_diff>
--- a/hallituspalaute.xlsx
+++ b/hallituspalaute.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
   <si>
     <t>moi 1.4.2017 @ 20:0</t>
   </si>
@@ -23,6 +23,9 @@
   </si>
   <si>
     <t>En tykkää :( 10.4.2017 @ 14:4</t>
+  </si>
+  <si>
+    <t>Moi 10.4.2017 @ 14:49</t>
   </si>
 </sst>
 </file>
@@ -370,7 +373,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:A4"/>
+  <dimension ref="A2:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
@@ -393,6 +396,11 @@
         <v>2</v>
       </c>
     </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Lisätty /raportti, jolla botti tulostaa viisi viimeisintä hallituspalautetta
</commit_message>
<xml_diff>
--- a/hallituspalaute.xlsx
+++ b/hallituspalaute.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samu\Documents\koodi\TGbot\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10368"/>
   </bookViews>
   <sheets>
-    <sheet name="Taul1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Taul1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>moi 1.4.2017 @ 20:0</t>
   </si>
@@ -27,24 +32,26 @@
   <si>
     <t>Moi 10.4.2017 @ 14:49</t>
   </si>
+  <si>
+    <t>asd</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -60,15 +67,24 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normaali" xfId="0"/>
+    <cellStyle name="Normaali" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -368,40 +384,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A2:A5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Hallituspalautteen raportointi toimii. Lisätty myös automaattinen palautelokin siistintä
</commit_message>
<xml_diff>
--- a/hallituspalaute.xlsx
+++ b/hallituspalaute.xlsx
@@ -9,33 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10368"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="6132" windowHeight="7008"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>moi 1.4.2017 @ 20:0</t>
-  </si>
-  <si>
-    <t>Testi 7.4.2017 @ 21:47</t>
-  </si>
-  <si>
-    <t>En tykkää :( 10.4.2017 @ 14:4</t>
-  </si>
-  <si>
-    <t>Moi 10.4.2017 @ 14:49</t>
-  </si>
-  <si>
-    <t>asd</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -385,37 +365,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:A6"/>
+  <dimension ref="A2:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A28" sqref="A4:A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
+      <c r="A2">
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>4</v>
+      <c r="A3">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Koodia kommentoitu ja siistitty.
</commit_message>
<xml_diff>
--- a/hallituspalaute.xlsx
+++ b/hallituspalaute.xlsx
@@ -365,25 +365,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:A3"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A28" sqref="A4:A28"/>
+      <selection activeCell="C25" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>53</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
palautesheet pommitettu rikki, katso mitä sisältää
</commit_message>
<xml_diff>
--- a/hallituspalaute.xlsx
+++ b/hallituspalaute.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
   <si>
     <t>Moi! @ 10.4.2017, 20:39</t>
   </si>
@@ -56,6 +56,55 @@
   </si>
   <si>
     <t>" return 0" @ 10.5.2017, 16:57</t>
+  </si>
+  <si>
+    <t>The Project Gutenberg EBook of The Adventures of Sherlock Holmes
+by Sir Arthur Conan Doyle
+(#15 in our series by Sir Arthur Conan Doyle)
+Copyright laws are changing all over the world. Be sure to check the
+copyright laws for your country before downloading or redistributing
+this or any other Project Gutenberg eBook.
+This header should be the first thing seen when viewing this Project
+Gutenberg file.  Please do not remove it.  Do not change or edit the
+header without written permission.
+Please read the "legal small print," and other information about the
+eBook and Project Gutenberg at the bottom of this file.  Included is
+important information about your specific rights and restrictions in
+how the file may be used.  You can also find out about how to make a
+donation to Project Gutenberg, and how to get involved.
+Welcome To The World of Free Plain Vanilla Electronic Texts
+eBooks Readable By Both Humans and By Computers, Since 1971
+***These eBooks Were Prepared By Thousands of Volunteers!***
+Title: The Adventures of Sherlock Holmes
+Author: Sir Arthur Conan Doyle
+Release Date: March, 1999  [EBook #1661]
+[Most recently updated: November 29, 2002]
+Edition: 12
+Language: English
+Character set encoding: ASCII
+* START OF THE PROJECT GUTENBERG EBOOK, THE ADVENTURES OF SHERLOCK HOLMES *
+(Additional editing by Jose Menendez)
+THE ADVENTURES OF
+SHERLOCK HOLMES
+BY
+SIR ARTHUR CONAN DOYLE
+CONTENTS
+I.    A Scandal in Bohemia
+II.    The Red-Headed League
+III.    A Case of Identity
+IV.    The Boscombe Valley Mystery
+V.    The Five Orange Pips
+VI.    The Man with the Twisted Lip
+VII.    The Adventure of the Blue Carbuncle
+VIII.    The Adventure of the Speckled Band
+IX.    The Adventure of the Engineer's Thumb
+X.    The Adventure of the Noble Bachelor
+XI.    The Adventure of the Beryl Coronet
+XII.    The Adventure of the Copper Beeches
+ADVENTURE  I.  A SCANDAL IN BOHEMIA
+I.
+To Sherlock Holmes she is always the woman. I have seldom heard him mention her under any other name. In his eyes she eclipses and predominates the whole of her sex. It was not that he felt any emotion akin to love for Irene Adler. All emotions, and that one particularly, were abhorrent to his cold, precise but admirably balanced mind. He was, I take it, the most perfect reasoning and observing machine that the world has seen, but as a lover he would have placed himself in a false position. He never spoke of the softer passions, save with a gibe and a sneer. They were admirable things for the observer--excellent for drawing the veil from men's motives and actions. But for the trained reasoner to admit such intrusions into his own delicate and finely adjusted temperament was to introduce a distracting factor which might throw a doubt upon all his mental results. Grit in a sensitive instrument, or a crack in one of his own high-power lenses, would not be more disturbing than a strong emotion in a nature such as his. And yet there was but one woman to him, and that woman was the late Irene Adler, of dubious and questionable memory.
+I had seen little of Holmes lately. My marriage had drifted us away from each other. My own complete happiness, and the home-centred interests which rise up around the man who first finds himself master of his own establishment, were sufficient to absorb all my attention, while Holmes, who loathed every form of society with his whole Bohemian soul, remained in our lodgings in Baker Street, buried among his old books, and alternating from week to week between cocaine and ambition, the drowsiness of the drug, and the fierce energy of his own keen nature. He was still, as ever, deeply attracted by the study of crime, and occupied his immense faculties and extraordinary powers of observation in following out those clues, and clearing up those mysteries which had been abandoned as hopeless by the official police. From time to time I heard some vague account of his doings: of his summons to Odessa in the case of the Trepoff murder, of his clearing up of the singular tragedy of the Atkinson brothers at Trinco @ 10.5.2017, 17:6</t>
   </si>
 </sst>
 </file>
@@ -403,7 +452,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:A15"/>
+  <dimension ref="A2:A16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
       <selection activeCell="C25" sqref="A1:XFD1048576"/>
@@ -481,6 +530,11 @@
         <v>13</v>
       </c>
     </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Palautteen maksimipituuden tarkistus lisätty.
</commit_message>
<xml_diff>
--- a/hallituspalaute.xlsx
+++ b/hallituspalaute.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
   <si>
     <t>Moi! @ 10.4.2017, 20:39</t>
   </si>
@@ -37,74 +37,7 @@
     <t>Palaute! @ 11.4.2017, 16:32</t>
   </si>
   <si>
-    <t>Ä @ 10.5.2017, 16:51</t>
-  </si>
-  <si>
-    <t>Тслвдвдфжжфдплплпд/n @ 10.5.2017, 16:53</t>
-  </si>
-  <si>
-    <t>Æääääää @ 10.5.2017, 16:54</t>
-  </si>
-  <si>
-    <t>Äääöääläööääödjekjbdkdkdödäädösöäaååååååapakfkrkdkwnsjsk @ 10.5.2017, 16:54</t>
-  </si>
-  <si>
-    <t>😘 @ 10.5.2017, 16:55</t>
-  </si>
-  <si>
-    <t>💋 @ 10.5.2017, 16:55</t>
-  </si>
-  <si>
-    <t>" return 0" @ 10.5.2017, 16:57</t>
-  </si>
-  <si>
-    <t>The Project Gutenberg EBook of The Adventures of Sherlock Holmes
-by Sir Arthur Conan Doyle
-(#15 in our series by Sir Arthur Conan Doyle)
-Copyright laws are changing all over the world. Be sure to check the
-copyright laws for your country before downloading or redistributing
-this or any other Project Gutenberg eBook.
-This header should be the first thing seen when viewing this Project
-Gutenberg file.  Please do not remove it.  Do not change or edit the
-header without written permission.
-Please read the "legal small print," and other information about the
-eBook and Project Gutenberg at the bottom of this file.  Included is
-important information about your specific rights and restrictions in
-how the file may be used.  You can also find out about how to make a
-donation to Project Gutenberg, and how to get involved.
-Welcome To The World of Free Plain Vanilla Electronic Texts
-eBooks Readable By Both Humans and By Computers, Since 1971
-***These eBooks Were Prepared By Thousands of Volunteers!***
-Title: The Adventures of Sherlock Holmes
-Author: Sir Arthur Conan Doyle
-Release Date: March, 1999  [EBook #1661]
-[Most recently updated: November 29, 2002]
-Edition: 12
-Language: English
-Character set encoding: ASCII
-* START OF THE PROJECT GUTENBERG EBOOK, THE ADVENTURES OF SHERLOCK HOLMES *
-(Additional editing by Jose Menendez)
-THE ADVENTURES OF
-SHERLOCK HOLMES
-BY
-SIR ARTHUR CONAN DOYLE
-CONTENTS
-I.    A Scandal in Bohemia
-II.    The Red-Headed League
-III.    A Case of Identity
-IV.    The Boscombe Valley Mystery
-V.    The Five Orange Pips
-VI.    The Man with the Twisted Lip
-VII.    The Adventure of the Blue Carbuncle
-VIII.    The Adventure of the Speckled Band
-IX.    The Adventure of the Engineer's Thumb
-X.    The Adventure of the Noble Bachelor
-XI.    The Adventure of the Beryl Coronet
-XII.    The Adventure of the Copper Beeches
-ADVENTURE  I.  A SCANDAL IN BOHEMIA
-I.
-To Sherlock Holmes she is always the woman. I have seldom heard him mention her under any other name. In his eyes she eclipses and predominates the whole of her sex. It was not that he felt any emotion akin to love for Irene Adler. All emotions, and that one particularly, were abhorrent to his cold, precise but admirably balanced mind. He was, I take it, the most perfect reasoning and observing machine that the world has seen, but as a lover he would have placed himself in a false position. He never spoke of the softer passions, save with a gibe and a sneer. They were admirable things for the observer--excellent for drawing the veil from men's motives and actions. But for the trained reasoner to admit such intrusions into his own delicate and finely adjusted temperament was to introduce a distracting factor which might throw a doubt upon all his mental results. Grit in a sensitive instrument, or a crack in one of his own high-power lenses, would not be more disturbing than a strong emotion in a nature such as his. And yet there was but one woman to him, and that woman was the late Irene Adler, of dubious and questionable memory.
-I had seen little of Holmes lately. My marriage had drifted us away from each other. My own complete happiness, and the home-centred interests which rise up around the man who first finds himself master of his own establishment, were sufficient to absorb all my attention, while Holmes, who loathed every form of society with his whole Bohemian soul, remained in our lodgings in Baker Street, buried among his old books, and alternating from week to week between cocaine and ambition, the drowsiness of the drug, and the fierce energy of his own keen nature. He was still, as ever, deeply attracted by the study of crime, and occupied his immense faculties and extraordinary powers of observation in following out those clues, and clearing up those mysteries which had been abandoned as hopeless by the official police. From time to time I heard some vague account of his doings: of his summons to Odessa in the case of the Trepoff murder, of his clearing up of the singular tragedy of the Atkinson brothers at Trinco @ 10.5.2017, 17:6</t>
+    <t>b'Moro!' @ 10.5.2017, 20:54</t>
   </si>
 </sst>
 </file>
@@ -452,13 +385,16 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:A16"/>
+  <dimension ref="A2:A9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C25" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="98.6640625"/>
+  </cols>
   <sheetData>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
@@ -500,41 +436,6 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16" t="s">
-        <v>14</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>